<commit_message>
[ADD] Se unieron cambios de alan
</commit_message>
<xml_diff>
--- a/web-interface/resultados.xlsx
+++ b/web-interface/resultados.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,25 +442,25 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Maestra</v>
+        <v>Terapeuta</v>
       </c>
       <c r="B2" t="str">
-        <v>Asociación Centro de T...</v>
+        <v>La empresa es confidencial o no se encuentra disponible</v>
       </c>
       <c r="C2" t="str">
-        <v>SLP.</v>
+        <v>León,, Gto.</v>
       </c>
       <c r="D2" t="str">
-        <v>$5,000 - $6,000 Mensual</v>
+        <v>$14,000 - $16,000 Mensual</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="str">
-        <v>Educación</v>
+        <v>Sector salud</v>
       </c>
       <c r="G2" t="str">
-        <v>Educación especial</v>
+        <v>Terapeuta</v>
       </c>
       <c r="H2" t="str">
         <v>Universitario titulado</v>
@@ -469,12 +469,68 @@
         <v>Permanente</v>
       </c>
       <c r="J2" t="str">
+        <v>Tiempo completo</v>
+      </c>
+      <c r="K2" t="str">
+        <v>Presencial</v>
+      </c>
+      <c r="L2" t="str" xml:space="preserve">
+        <v xml:space="preserve">Requisitos del puesto
+Estudios universitarios con título en Terapia.
+Experiencia previa como Terapeuta de niños con Trastornos del espectro autista.
+Gusto por realizar manualidades.
+Habilidad para nadar.
+Licencia de manejo vigente.
+Conocimientos en técnicas de terapia y rehabilitación.
+Licencia o certificación válida en Terapia (deseable).
+Responsabilidades del puesto
+Realizar evaluaciones y diagnósticos de los pacientes.
+Diseñar planes de tratamiento personalizados.
+Realizar sesiones de terapia adaptadas a las necesidades individuales de cada paciente.
+Mantener registros precisos de la evolución de los pacientes.
+Prestaciones y beneficios adicionales
+Salario mensual competitivo de 14000 a 16000.
+Prestaciones de ley.
+Vales de despensa.
+Fondo de ahorro.
+Oportunidades de capacitación y desarrollo profesional en un ambiente de trabajo colaborativo y en constante crecimiento.</v>
+      </c>
+    </row>
+    <row r="3" xml:space="preserve">
+      <c r="A3" t="str">
+        <v>Maestra</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Asociación Centro de T...</v>
+      </c>
+      <c r="C3" t="str">
+        <v>SLP.</v>
+      </c>
+      <c r="D3" t="str">
+        <v>$5,000 - $6,000 Mensual</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Educación</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Educación especial</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Universitario titulado</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Permanente</v>
+      </c>
+      <c r="J3" t="str">
         <v>Medio tiempo</v>
       </c>
-      <c r="K2" t="str">
+      <c r="K3" t="str">
         <v>Híbrido</v>
       </c>
-      <c r="L2" t="str" xml:space="preserve">
+      <c r="L3" t="str" xml:space="preserve">
         <v xml:space="preserve">Acerca de la empresa
 **** Asociación Centro de Terapia Infantil y de Educación Especial es una organización comprometida con el bienestar y desarrollo de niños, niñas y jóvenes con autismo, síndrome de Down y/o discapacidad intelectual. Nuestra misión es brindar un ambiente inclusivo y terapéutico para promover su crecimiento y aprendizaje. - **Ubicación:** San Luis Potosí.
 Requisitos del puesto
@@ -494,41 +550,41 @@
 Ambiente de trabajo colaborativo y respetuoso.</v>
       </c>
     </row>
-    <row r="3" xml:space="preserve">
-      <c r="A3" t="str">
+    <row r="4" xml:space="preserve">
+      <c r="A4" t="str">
         <v>Monitora en inclusión educativa (maestro sombra)</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B4" t="str">
         <v>CC INTEGRACION LABORAL</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C4" t="str">
         <v>CDMX</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D4" t="str">
         <v>$8,500 Mensual</v>
       </c>
-      <c r="E3" t="b">
+      <c r="E4" t="b">
         <v>0</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F4" t="str">
         <v>Educación</v>
       </c>
-      <c r="G3" t="str">
+      <c r="G4" t="str">
         <v>Educación especial</v>
       </c>
-      <c r="H3" t="str">
+      <c r="H4" t="str">
         <v>Universitario sin titulo</v>
       </c>
-      <c r="I3" t="str">
+      <c r="I4" t="str">
         <v>Permanente</v>
       </c>
-      <c r="J3" t="str">
+      <c r="J4" t="str">
         <v>Tiempo completo</v>
       </c>
-      <c r="K3" t="str">
+      <c r="K4" t="str">
         <v>Presencial</v>
       </c>
-      <c r="L3" t="str" xml:space="preserve">
+      <c r="L4" t="str" xml:space="preserve">
         <v xml:space="preserve">REQUISITOS:
 Nivel de estudios: Licenciatura (concluida o últimos semestres) Psicología educativa, Pedagogía, Educación especial o afines
 23 a 32 años
@@ -544,165 +600,9 @@
 Interesados enviar cv a la dirección de contacto.</v>
       </c>
     </row>
-    <row r="4" xml:space="preserve">
-      <c r="A4" t="str">
-        <v>TERAPEUTA ESPECIALIZADA EN TEA Y TDAH</v>
-      </c>
-      <c r="B4" t="str">
-        <v>La empresa es confidencial o no se encuentra disponible</v>
-      </c>
-      <c r="C4" t="str">
-        <v>CDMX</v>
-      </c>
-      <c r="D4" t="str">
-        <v>$9,000 - $12,000 Mensual</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Ciencias sociales - Humanidades</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Psicología</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Universitario sin titulo</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Permanente</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Tiempo completo</v>
-      </c>
-      <c r="K4" t="str">
-        <v>Presencial</v>
-      </c>
-      <c r="L4" t="str" xml:space="preserve">
-        <v xml:space="preserve">TERAPEUTA ESPECIALIZADA EN TEA Y TDAH
-Fundación Valentina – Benito Juárez, Ciudad de México, Anaxágoras 25, Col. Piedad Narvarte, Alcaldía Benito Juárez, CDMX.
-Horario: Lunes a viernes de 8:30 a 18:00 hrs
-Sueldo: $9,000 a $12,000 mensuales (según experiencia)
-OBJETIVO DEL PUESTO
-Brindar atención terapéutica especializada a niños, niñas y adolescentes con diagnóstico de Trastorno del Espectro Autista (TEA) y/o Trastorno por Déficit de Atención e Hiperactividad (TDAH), mediante un enfoque individualizado que favorezca su desarrollo integral, habilidades sociales, comunicación, autorregulación y autonomía.
-PERFIL REQUERIDO
-Sexo: Femenino
-Edad: 25 a 30 años
-Escolaridad: Licenciatura en Psicología (PRINCIPALEMENTE PSICOLOGIA CLINICA), Psicopedagogía, Pedagogía o Terapia Ocupacional, con especialidad o formación en educación especial, neurodiversidad o neurociencias (Indispensable contar con título y cédula profesional o en proceso).
-Formación adicional deseable: Diplomados o certificaciones en ABA, PECS, TEACCH, Denver o afines.
-Experiencia mínima: 1 año comprobable trabajando con población TEA y/o TDAH.
-Residencia: No vivir a más de una hora de distancia del centro.
-HABILIDADES CLAVES
-Saber realizar diagnósticos y valoraciones en TEA y TDAH. ?
-Diseño e implementación de planes terapéuticos individuales.
-Elaboración de bitácoras y reportes terapéuticos.
-Trabajo colaborativo y orientación a familias.
-Alta empatía, responsabilidad, comunicación y observación clínica.
-FUNCIONES PRINCIPALES
-Realización de valoraciones y diagnósticos clínico-funcionales en TEA y TDAH.
-Diseño y aplicación de intervenciones personalizadas.
-Elaboración y entrega mensual de planeaciones terapéuticas.
-Registro y envío de bitácoras mensuales.
-Aplicación de técnicas conductuales y metodologías estructuradas.
-Trabajo coordinado con equipo multidisciplinario.
-Asesoramiento continuo a padres de familia.
-SOLO POSTULARSE SI CUMPLES CON LOS REQUISITOS DEL PERFIL, SOLO PSICOLOGAS CLINICAS ESPECIALIZADAS EN TEA Y TDAH, NO LABORALES</v>
-      </c>
-    </row>
-    <row r="5" xml:space="preserve">
-      <c r="A5" t="str">
-        <v>Closer SaaS B2B Startup Tecnologica</v>
-      </c>
-      <c r="B5" t="str">
-        <v>La empresa es confidencial o no se encuentra disponible</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Torreón,, Coah.</v>
-      </c>
-      <c r="D5" t="str">
-        <v>$20,000 - $25,000 Mensual</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Ventas</v>
-      </c>
-      <c r="G5" t="str">
-        <v>Comercial</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Universitario titulado</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Permanente</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Tiempo completo</v>
-      </c>
-      <c r="K5" t="str">
-        <v>Híbrido</v>
-      </c>
-      <c r="L5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Empresa:
-SuperLeads — Plataforma SaaS que impulsa las admisiones y la matrícula de instituciones educativas en Latinoamérica mediante tecnología inteligente y procesos comerciales impecables.
-Objetivo del rol
-Ser la primera línea de crecimiento de SuperLeads: realizar prospección outbound diaria (llamadas, correos y LinkedIn) a nuestro *Ideal Customer Profile* (ICP) para generar al menos 30 conexiones efectivas por día y agendar citas calificadas para nuestro equipo de Account Executives.
-Responsabilidades clave
-Ejecutar cadencias multicanal (teléfono, email, LinkedIn) y mantener registro de todo en SuperLeads &lt;- Usas el mejor CRM para vender el mejor CRM educativo, tu capacitación de explicación esta intimamente ligada a tu uso del CRM para vender!
-Detectar necesidades, calificar leads con criterio Bajo, Medio, Alto y concertar reuniones.
-Alcanzar meta semanal de citas asistidas y tasa de respuesta mínima del 15 %.
-Colaborar con Marketing para nutrir leads y con Closers para retroalimentación de calidad.
-Participar en role-plays, coaching, Talleres, Congresos y workshops internos para elevar tu pitch.
-Representar la cultura SuperLeads: presencia real, comunicación consciente y ritmo sostenible.
-Compensación
-Sueldo base: $12,000 MXN brutos/mes
-De $500 MXN a $5,000 MXN por cada cita calificada que se lleve a cabo.
-Ingreso estimado: $40,000 MXN/mes (base + comisiones). &lt;- Buscamos solo gente responsable
-Prestaciones de ley, laptop y línea telefónica corporativa.
-Requisitos
-5 + año en prospección o telemarketing B2B (ventas SaaS o educación, deseable).
-Dominio de llamadas en frío (que no te de miedo ni flojera), redacción de correos y social-selling en LinkedIn, que te guste escribir.
-Conocimiento básico de CRM (HubSpot o similar) y hábito de documentación rigurosa.
-Actitud hunter (eres un cazador y no paras hasta lograr la cita), resiliencia ante la objeción y enfoque a métricas diarias.
-Excelente ortografía y dicción; gusto por aprender y aportar ideas.
-Disponibilidad tiempo completo en oficina de Torreón.
-Lo que ofrecemos
-Plan de carrera claro a Closer en 12-18 meses según performance.
-Formación continua en metodologías de venta consultiva (SPIN, MEDDICC, Challenger).
-Ambiente de alto desempeño con calidez humana: celebramos logros y cuidamos el bienestar.
-Propósito de impacto: ayudar a colegios y universidades a transformar sus admisiones.
----
-¿Te apasiona la prospección, el contacto humano y el mundo EdTech?
-¡Únete a SuperLeads y conviértete en la chispa que encienda el crecimiento educativo en LATAM!
-Tipo de puesto: Tiempo completo
-Sueldo: A partir de $12,000 MXN al mes &lt;- Esto es el inicial, si no ganas 3 veces más esto al menos, te descontraríamos por que nos hacemos daño, nos gusta que las personas con nosotros gane bien y esto lo demuestra.
-Beneficios:
-Aumentos salariales ritmo Startup
-Días de paternidad superiores a los de la ley
-Laptop y celular de la empresa
-&gt;100 Ventas, Carro de la empresa
-Pago complementario:
-Bono anual &gt;52 ventas en el año
-Bono de productividad Pago por Cita asistida
-Tipo de jornada:
-55 horas semanales mínimo
-Como tu las acomodes
-Pregunta(s) de postulación: (Es importante que tengamos estas respuestas.
-Describe en 2-3 líneas tu logro laboral más sobresaliente
-Si te contratamos, ¿cómo serían tus primeros 100 días en SuperLeads?
-¿Tu puesto como impacta directamente los ingresos de la empresa, exactamente?
-Lugar de trabajo: Empleo presencial o Híbrido.
-Fecha de inicio prevista: 01/08/2025
-Solo aplica si crees que eres Player A, osea un Mini-Ceo, entrepeneur, Motivado siempre, Con deficit de atención, Autismo.
-Nos vemos pronto ó no.
-Ing. Ricardo López Reyero
-Founder Comercial SuperLeads</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>